<commit_message>
Newly updated with tables fixed
</commit_message>
<xml_diff>
--- a/tables/1972-73/1972-73_Table3.xlsx
+++ b/tables/1972-73/1972-73_Table3.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dolaosebikan\Desktop\iita cassava reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/m_adetuyi_cgiar_org/Documents/WORK/MR PRASAD/2022/7. August/Annual Report/New_Tables/1972-73/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8610" windowHeight="5805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8610" windowHeight="5805"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Degree of Cynaogenesis</t>
   </si>
@@ -51,15 +50,26 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Table 3: Degree of cyanogenesis in cassava leaf discs</t>
+    <t>Table Name:</t>
+  </si>
+  <si>
+    <t>Degree of cyanogenesis in cassava leaf discs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -83,13 +93,139 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,68 +519,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>87747</v>
-      </c>
-      <c r="C2">
-        <v>99.14</v>
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>671</v>
-      </c>
-      <c r="C3">
-        <v>0.76</v>
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>87747</v>
+      </c>
+      <c r="C3" s="5">
+        <v>99.14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>92</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>671</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>92</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="9">
         <v>88510</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="10">
         <v>100</v>
       </c>
     </row>
@@ -453,22 +598,290 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100284A27838130D149A2783A40AB43BA83" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bac4f5e4b6cdcb97fbf92ed416088beb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1ef7e49f-bd9c-470c-bea7-6795de71c18b" xmlns:ns4="1ce501d2-3302-407b-b8e4-287cbb5596d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b7d79c94ab8e42cd9b5996806927073" ns3:_="" ns4:_="">
+    <xsd:import namespace="1ef7e49f-bd9c-470c-bea7-6795de71c18b"/>
+    <xsd:import namespace="1ce501d2-3302-407b-b8e4-287cbb5596d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1ef7e49f-bd9c-470c-bea7-6795de71c18b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1ce501d2-3302-407b-b8e4-287cbb5596d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="21" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B5F4A1B-8364-491B-B211-564211A87346}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1ef7e49f-bd9c-470c-bea7-6795de71c18b"/>
+    <ds:schemaRef ds:uri="1ce501d2-3302-407b-b8e4-287cbb5596d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA4A7F4-595D-4534-99FB-9B479C31D52F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA6B15C6-F1A2-4BFB-8859-455F4CAEFD07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1ef7e49f-bd9c-470c-bea7-6795de71c18b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1ce501d2-3302-407b-b8e4-287cbb5596d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>